<commit_message>
code to add general information to Excel files
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13776,8 +13776,8 @@
       <c r="A2" s="295" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="377" t="s">
-        <v>263</v>
+      <c r="F2" s="377" t="str">
+        <v>EnergyPlus 8.6.0</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -13795,8 +13795,8 @@
       <c r="G3" s="349"/>
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
-      <c r="J3" s="360">
-        <v>39814</v>
+      <c r="J3" s="360" t="str">
+        <v>9//30/2016</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13813,8 +13813,8 @@
       <c r="G4" s="349"/>
       <c r="H4" s="349"/>
       <c r="I4" s="349"/>
-      <c r="J4" s="350" t="s">
-        <v>264</v>
+      <c r="J4" s="350" t="str">
+        <v>E+</v>
       </c>
       <c r="K4" s="108" t="s">
         <v>56</v>
@@ -13834,8 +13834,8 @@
       <c r="G5" s="349"/>
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
-      <c r="J5" s="360">
-        <v>40179</v>
+      <c r="J5" s="360" t="str">
+        <v>11/1/2016</v>
       </c>
       <c r="K5" s="109"/>
     </row>
@@ -13862,8 +13862,8 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="377" t="s">
-        <v>265</v>
+      <c r="F7" s="377" t="str">
+        <v>National Renewable Energy Laboratory</v>
       </c>
       <c r="G7" s="378"/>
       <c r="H7" s="378"/>
@@ -13883,8 +13883,8 @@
       <c r="G8" s="349"/>
       <c r="H8" s="349"/>
       <c r="I8" s="349"/>
-      <c r="J8" s="350" t="s">
-        <v>266</v>
+      <c r="J8" s="350" t="str">
+        <v>NREL</v>
       </c>
       <c r="K8" s="109"/>
     </row>

</xml_diff>

<commit_message>
Finished Updates for EP 8.7 and OS 2.1.0 results
Add copy of Excel Results files with OpenStudio program info
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13796,7 +13796,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>3//30/2017</v>
+        <v>3/30/2017</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -14116,7 +14116,7 @@
         <v>116</v>
       </c>
       <c r="B25" s="13">
-        <v>31.189</v>
+        <v>31.226</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -14146,7 +14146,7 @@
         <v>118</v>
       </c>
       <c r="B27" s="13">
-        <v>31.189</v>
+        <v>31.226</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -14344,7 +14344,7 @@
         <v>116</v>
       </c>
       <c r="B41" s="13">
-        <v>38.68</v>
+        <v>37.31</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -14374,7 +14374,7 @@
         <v>118</v>
       </c>
       <c r="B43" s="13">
-        <v>38.68</v>
+        <v>37.31</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -14572,7 +14572,7 @@
         <v>116</v>
       </c>
       <c r="B57" s="5">
-        <v>0.0001309021009313407</v>
+        <v>0.00012626570283734027</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -14602,7 +14602,7 @@
         <v>118</v>
       </c>
       <c r="B59" s="5">
-        <v>0.0001309021009313407</v>
+        <v>0.00012626570283734027</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -14725,7 +14725,7 @@
         <v>116</v>
       </c>
       <c r="B68" s="244">
-        <v>172.22222222222223</v>
+        <v>433.3333333333333</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -14755,7 +14755,7 @@
         <v>118</v>
       </c>
       <c r="B70" s="244">
-        <v>213.88888888888889</v>
+        <v>475.0</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>

</xml_diff>